<commit_message>
Now takes the schedule correctly. Generates weekly file and updates the output fiel for use in dashboard.
</commit_message>
<xml_diff>
--- a/nfl_current_week_schedule.xlsx
+++ b/nfl_current_week_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\offic\PycharmProjects\NFL Weekly Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F0232C-4486-4668-B294-659EE9D570E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180338A3-E4FE-44C6-94C4-C4EA652AA70C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Teams</t>
   </si>
@@ -31,115 +31,106 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Baltimore  @  Kansas City</t>
-  </si>
-  <si>
-    <t>Pittsburgh  @  Atlanta</t>
-  </si>
-  <si>
-    <t>Arizona  @  Buffalo</t>
-  </si>
-  <si>
-    <t>Tennessee  @  Chicago</t>
-  </si>
-  <si>
-    <t>New England  @  Cincinnati</t>
-  </si>
-  <si>
-    <t>Houston  @  Indianapolis</t>
-  </si>
-  <si>
-    <t>Jacksonville  @  Miami</t>
-  </si>
-  <si>
-    <t>Carolina  @  New Orleans</t>
-  </si>
-  <si>
-    <t>Minnesota  @  NY Giants</t>
-  </si>
-  <si>
-    <t>Las Vegas  @  LA Chargers</t>
-  </si>
-  <si>
-    <t>Denver  @  Seattle</t>
-  </si>
-  <si>
-    <t>Dallas  @  Cleveland</t>
-  </si>
-  <si>
-    <t>Washington  @  Tampa Bay</t>
-  </si>
-  <si>
-    <t>LA Rams  @  Detroit</t>
-  </si>
-  <si>
-    <t>NY Jets  @  San Francisco</t>
+    <t>Tampa Bay  @  Atlanta</t>
+  </si>
+  <si>
+    <t>Cleveland  @  Washington</t>
+  </si>
+  <si>
+    <t>Indianapolis  @  Jacksonville</t>
+  </si>
+  <si>
+    <t>Miami  @  New England</t>
+  </si>
+  <si>
+    <t>Buffalo  @  Houston</t>
+  </si>
+  <si>
+    <t>Baltimore  @  Cincinnati</t>
+  </si>
+  <si>
+    <t>Carolina  @  Chicago</t>
+  </si>
+  <si>
+    <t>Las Vegas  @  Denver</t>
+  </si>
+  <si>
+    <t>Arizona  @  San Francisco</t>
+  </si>
+  <si>
+    <t>Green Bay  @  LA Rams</t>
+  </si>
+  <si>
+    <t>NY Giants  @  Seattle</t>
+  </si>
+  <si>
+    <t>Dallas  @  Pittsburgh</t>
+  </si>
+  <si>
+    <t>New Orleans  @  Kansas City</t>
+  </si>
+  <si>
+    <t>8:15 PM</t>
+  </si>
+  <si>
+    <t>9:30 AM</t>
+  </si>
+  <si>
+    <t>1:00 PM</t>
+  </si>
+  <si>
+    <t>4:05 PM</t>
+  </si>
+  <si>
+    <t>4:25 PM</t>
   </si>
   <si>
     <t>8:20 PM</t>
   </si>
   <si>
-    <t>8:15 PM</t>
-  </si>
-  <si>
-    <t>1:00 PM</t>
-  </si>
-  <si>
-    <t>4:05 PM</t>
-  </si>
-  <si>
-    <t>4:25 PM</t>
+    <t>Mercedes-Benz Stadium</t>
+  </si>
+  <si>
+    <t>Tottenham Hotspur Stadium</t>
+  </si>
+  <si>
+    <t>Northwest Stadium</t>
+  </si>
+  <si>
+    <t>EverBank Stadium</t>
+  </si>
+  <si>
+    <t>Gillette Stadium</t>
+  </si>
+  <si>
+    <t>NRG Stadium</t>
+  </si>
+  <si>
+    <t>Paycor Stadium</t>
+  </si>
+  <si>
+    <t>Soldier Field</t>
+  </si>
+  <si>
+    <t>Empower Field at Mile High</t>
+  </si>
+  <si>
+    <t>Levi's Stadium</t>
+  </si>
+  <si>
+    <t>SoFi Stadium</t>
+  </si>
+  <si>
+    <t>Lumen Field</t>
+  </si>
+  <si>
+    <t>Acrisure Stadium</t>
   </si>
   <si>
     <t>GEHA Field at Arrowhead Stadium</t>
   </si>
   <si>
-    <t>Corinthians Arena</t>
-  </si>
-  <si>
-    <t>Mercedes-Benz Stadium</t>
-  </si>
-  <si>
-    <t>Highmark Stadium</t>
-  </si>
-  <si>
-    <t>Soldier Field</t>
-  </si>
-  <si>
-    <t>Paycor Stadium</t>
-  </si>
-  <si>
-    <t>Lucas Oil Stadium</t>
-  </si>
-  <si>
-    <t>Hard Rock Stadium</t>
-  </si>
-  <si>
-    <t>Caesars Superdome</t>
-  </si>
-  <si>
-    <t>MetLife Stadium</t>
-  </si>
-  <si>
-    <t>SoFi Stadium</t>
-  </si>
-  <si>
-    <t>Lumen Field</t>
-  </si>
-  <si>
-    <t>Huntington Bank Field</t>
-  </si>
-  <si>
-    <t>Raymond James Stadium</t>
-  </si>
-  <si>
-    <t>Ford Field</t>
-  </si>
-  <si>
-    <t>Levi's Stadium</t>
-  </si>
-  <si>
-    <t>Green Bay  @  Philadelphia</t>
+    <t>NY Jets  vs.  Minnesota</t>
   </si>
 </sst>
 </file>
@@ -541,15 +532,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -568,21 +559,21 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -590,10 +581,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -601,10 +592,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -612,10 +603,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -623,10 +614,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -634,10 +625,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -645,10 +636,10 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -656,10 +647,10 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -667,10 +658,10 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -678,10 +669,10 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -689,10 +680,10 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -700,10 +691,10 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -711,32 +702,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update for week 6
</commit_message>
<xml_diff>
--- a/nfl_current_week_schedule.xlsx
+++ b/nfl_current_week_schedule.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\offic\PycharmProjects\NFL Weekly Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180338A3-E4FE-44C6-94C4-C4EA652AA70C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Teams</t>
   </si>
@@ -31,43 +25,46 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Tampa Bay  @  Atlanta</t>
-  </si>
-  <si>
-    <t>Cleveland  @  Washington</t>
-  </si>
-  <si>
-    <t>Indianapolis  @  Jacksonville</t>
-  </si>
-  <si>
-    <t>Miami  @  New England</t>
-  </si>
-  <si>
-    <t>Buffalo  @  Houston</t>
-  </si>
-  <si>
-    <t>Baltimore  @  Cincinnati</t>
-  </si>
-  <si>
-    <t>Carolina  @  Chicago</t>
-  </si>
-  <si>
-    <t>Las Vegas  @  Denver</t>
-  </si>
-  <si>
-    <t>Arizona  @  San Francisco</t>
-  </si>
-  <si>
-    <t>Green Bay  @  LA Rams</t>
-  </si>
-  <si>
-    <t>NY Giants  @  Seattle</t>
-  </si>
-  <si>
-    <t>Dallas  @  Pittsburgh</t>
-  </si>
-  <si>
-    <t>New Orleans  @  Kansas City</t>
+    <t>San Francisco  @  Seattle</t>
+  </si>
+  <si>
+    <t>Jacksonville  vs.  Chicago</t>
+  </si>
+  <si>
+    <t>Indianapolis  @  Tennessee</t>
+  </si>
+  <si>
+    <t>Cleveland  @  Philadelphia</t>
+  </si>
+  <si>
+    <t>Tampa Bay  @  New Orleans</t>
+  </si>
+  <si>
+    <t>Houston  @  New England</t>
+  </si>
+  <si>
+    <t>Arizona  @  Green Bay</t>
+  </si>
+  <si>
+    <t>Washington  @  Baltimore</t>
+  </si>
+  <si>
+    <t>LA Chargers  @  Denver</t>
+  </si>
+  <si>
+    <t>Pittsburgh  @  Las Vegas</t>
+  </si>
+  <si>
+    <t>Atlanta  @  Carolina</t>
+  </si>
+  <si>
+    <t>Detroit  @  Dallas</t>
+  </si>
+  <si>
+    <t>Cincinnati  @  NY Giants</t>
+  </si>
+  <si>
+    <t>Buffalo  @  NY Jets</t>
   </si>
   <si>
     <t>8:15 PM</t>
@@ -88,56 +85,50 @@
     <t>8:20 PM</t>
   </si>
   <si>
-    <t>Mercedes-Benz Stadium</t>
+    <t>Lumen Field</t>
   </si>
   <si>
     <t>Tottenham Hotspur Stadium</t>
   </si>
   <si>
-    <t>Northwest Stadium</t>
-  </si>
-  <si>
-    <t>EverBank Stadium</t>
+    <t>Nissan Stadium</t>
+  </si>
+  <si>
+    <t>Lincoln Financial Field</t>
+  </si>
+  <si>
+    <t>Caesars Superdome</t>
   </si>
   <si>
     <t>Gillette Stadium</t>
   </si>
   <si>
-    <t>NRG Stadium</t>
-  </si>
-  <si>
-    <t>Paycor Stadium</t>
-  </si>
-  <si>
-    <t>Soldier Field</t>
+    <t>Lambeau Field</t>
+  </si>
+  <si>
+    <t>M&amp;T Bank Stadium</t>
   </si>
   <si>
     <t>Empower Field at Mile High</t>
   </si>
   <si>
-    <t>Levi's Stadium</t>
-  </si>
-  <si>
-    <t>SoFi Stadium</t>
-  </si>
-  <si>
-    <t>Lumen Field</t>
-  </si>
-  <si>
-    <t>Acrisure Stadium</t>
-  </si>
-  <si>
-    <t>GEHA Field at Arrowhead Stadium</t>
-  </si>
-  <si>
-    <t>NY Jets  vs.  Minnesota</t>
+    <t>Allegiant Stadium</t>
+  </si>
+  <si>
+    <t>Bank of America Stadium</t>
+  </si>
+  <si>
+    <t>AT&amp;T Stadium</t>
+  </si>
+  <si>
+    <t>MetLife Stadium</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,14 +191,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -254,7 +237,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -286,27 +269,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -338,24 +303,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -531,19 +478,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,155 +496,155 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B15" t="s">
         <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>16</v>
       </c>
       <c r="C15" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
added script for writing to gsheets and securing sensitive data
</commit_message>
<xml_diff>
--- a/nfl_current_week_schedule.xlsx
+++ b/nfl_current_week_schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>Teams</t>
   </si>
@@ -25,46 +25,49 @@
     <t>Location</t>
   </si>
   <si>
-    <t>San Francisco  @  Seattle</t>
-  </si>
-  <si>
-    <t>Jacksonville  vs.  Chicago</t>
-  </si>
-  <si>
-    <t>Indianapolis  @  Tennessee</t>
-  </si>
-  <si>
-    <t>Cleveland  @  Philadelphia</t>
-  </si>
-  <si>
-    <t>Tampa Bay  @  New Orleans</t>
-  </si>
-  <si>
-    <t>Houston  @  New England</t>
-  </si>
-  <si>
-    <t>Arizona  @  Green Bay</t>
-  </si>
-  <si>
-    <t>Washington  @  Baltimore</t>
-  </si>
-  <si>
-    <t>LA Chargers  @  Denver</t>
-  </si>
-  <si>
-    <t>Pittsburgh  @  Las Vegas</t>
-  </si>
-  <si>
-    <t>Atlanta  @  Carolina</t>
-  </si>
-  <si>
-    <t>Detroit  @  Dallas</t>
-  </si>
-  <si>
-    <t>Cincinnati  @  NY Giants</t>
-  </si>
-  <si>
-    <t>Buffalo  @  NY Jets</t>
+    <t>Denver  @  New Orleans</t>
+  </si>
+  <si>
+    <t>New England  vs.  Jacksonville</t>
+  </si>
+  <si>
+    <t>Philadelphia  @  NY Giants</t>
+  </si>
+  <si>
+    <t>Detroit  @  Minnesota</t>
+  </si>
+  <si>
+    <t>Miami  @  Indianapolis</t>
+  </si>
+  <si>
+    <t>Houston  @  Green Bay</t>
+  </si>
+  <si>
+    <t>Cincinnati  @  Cleveland</t>
+  </si>
+  <si>
+    <t>Tennessee  @  Buffalo</t>
+  </si>
+  <si>
+    <t>Seattle  @  Atlanta</t>
+  </si>
+  <si>
+    <t>Las Vegas  @  LA Rams</t>
+  </si>
+  <si>
+    <t>Carolina  @  Washington</t>
+  </si>
+  <si>
+    <t>Kansas City  @  San Francisco</t>
+  </si>
+  <si>
+    <t>NY Jets  @  Pittsburgh</t>
+  </si>
+  <si>
+    <t>Baltimore  @  Tampa Bay</t>
+  </si>
+  <si>
+    <t>LA Chargers  @  Arizona</t>
   </si>
   <si>
     <t>8:15 PM</t>
@@ -85,43 +88,52 @@
     <t>8:20 PM</t>
   </si>
   <si>
-    <t>Lumen Field</t>
-  </si>
-  <si>
-    <t>Tottenham Hotspur Stadium</t>
-  </si>
-  <si>
-    <t>Nissan Stadium</t>
-  </si>
-  <si>
-    <t>Lincoln Financial Field</t>
+    <t>9:00 PM</t>
   </si>
   <si>
     <t>Caesars Superdome</t>
   </si>
   <si>
-    <t>Gillette Stadium</t>
+    <t>Wembley Stadium</t>
+  </si>
+  <si>
+    <t>MetLife Stadium</t>
+  </si>
+  <si>
+    <t>U.S. Bank Stadium</t>
+  </si>
+  <si>
+    <t>Lucas Oil Stadium</t>
   </si>
   <si>
     <t>Lambeau Field</t>
   </si>
   <si>
-    <t>M&amp;T Bank Stadium</t>
-  </si>
-  <si>
-    <t>Empower Field at Mile High</t>
-  </si>
-  <si>
-    <t>Allegiant Stadium</t>
-  </si>
-  <si>
-    <t>Bank of America Stadium</t>
-  </si>
-  <si>
-    <t>AT&amp;T Stadium</t>
-  </si>
-  <si>
-    <t>MetLife Stadium</t>
+    <t>Huntington Bank Field</t>
+  </si>
+  <si>
+    <t>Highmark Stadium</t>
+  </si>
+  <si>
+    <t>Mercedes-Benz Stadium</t>
+  </si>
+  <si>
+    <t>SoFi Stadium</t>
+  </si>
+  <si>
+    <t>Northwest Stadium</t>
+  </si>
+  <si>
+    <t>Levi's Stadium</t>
+  </si>
+  <si>
+    <t>Acrisure Stadium</t>
+  </si>
+  <si>
+    <t>Raymond James Stadium</t>
+  </si>
+  <si>
+    <t>State Farm Stadium</t>
   </si>
 </sst>
 </file>
@@ -479,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -501,10 +513,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -512,10 +524,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -523,10 +535,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -534,10 +546,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -545,10 +557,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -556,10 +568,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -567,10 +579,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -578,10 +590,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -592,7 +604,7 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -600,10 +612,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -614,7 +626,7 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -622,10 +634,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -633,10 +645,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -644,10 +656,21 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="C15" t="s">
-        <v>35</v>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added logging for debugging purposes to all scripts. Renamed scripts for consistency
</commit_message>
<xml_diff>
--- a/nfl_current_week_schedule.xlsx
+++ b/nfl_current_week_schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>Teams</t>
   </si>
@@ -25,57 +25,57 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Denver  @  New Orleans</t>
-  </si>
-  <si>
-    <t>New England  vs.  Jacksonville</t>
-  </si>
-  <si>
-    <t>Philadelphia  @  NY Giants</t>
-  </si>
-  <si>
-    <t>Detroit  @  Minnesota</t>
-  </si>
-  <si>
-    <t>Miami  @  Indianapolis</t>
-  </si>
-  <si>
-    <t>Houston  @  Green Bay</t>
-  </si>
-  <si>
-    <t>Cincinnati  @  Cleveland</t>
-  </si>
-  <si>
-    <t>Tennessee  @  Buffalo</t>
-  </si>
-  <si>
-    <t>Seattle  @  Atlanta</t>
-  </si>
-  <si>
-    <t>Las Vegas  @  LA Rams</t>
-  </si>
-  <si>
-    <t>Carolina  @  Washington</t>
-  </si>
-  <si>
-    <t>Kansas City  @  San Francisco</t>
-  </si>
-  <si>
-    <t>NY Jets  @  Pittsburgh</t>
-  </si>
-  <si>
-    <t>Baltimore  @  Tampa Bay</t>
-  </si>
-  <si>
-    <t>LA Chargers  @  Arizona</t>
+    <t>Minnesota  @  LA Rams</t>
+  </si>
+  <si>
+    <t>Green Bay  @  Jacksonville</t>
+  </si>
+  <si>
+    <t>Atlanta  @  Tampa Bay</t>
+  </si>
+  <si>
+    <t>NY Jets  @  New England</t>
+  </si>
+  <si>
+    <t>Arizona  @  Miami</t>
+  </si>
+  <si>
+    <t>Indianapolis  @  Houston</t>
+  </si>
+  <si>
+    <t>Tennessee  @  Detroit</t>
+  </si>
+  <si>
+    <t>Baltimore  @  Cleveland</t>
+  </si>
+  <si>
+    <t>Philadelphia  @  Cincinnati</t>
+  </si>
+  <si>
+    <t>New Orleans  @  LA Chargers</t>
+  </si>
+  <si>
+    <t>Buffalo  @  Seattle</t>
+  </si>
+  <si>
+    <t>Kansas City  @  Las Vegas</t>
+  </si>
+  <si>
+    <t>Carolina  @  Denver</t>
+  </si>
+  <si>
+    <t>Chicago  @  Washington</t>
+  </si>
+  <si>
+    <t>Dallas  @  San Francisco</t>
+  </si>
+  <si>
+    <t>NY Giants  @  Pittsburgh</t>
   </si>
   <si>
     <t>8:15 PM</t>
   </si>
   <si>
-    <t>9:30 AM</t>
-  </si>
-  <si>
     <t>1:00 PM</t>
   </si>
   <si>
@@ -88,37 +88,40 @@
     <t>8:20 PM</t>
   </si>
   <si>
-    <t>9:00 PM</t>
-  </si>
-  <si>
-    <t>Caesars Superdome</t>
-  </si>
-  <si>
-    <t>Wembley Stadium</t>
-  </si>
-  <si>
-    <t>MetLife Stadium</t>
-  </si>
-  <si>
-    <t>U.S. Bank Stadium</t>
-  </si>
-  <si>
-    <t>Lucas Oil Stadium</t>
-  </si>
-  <si>
-    <t>Lambeau Field</t>
+    <t>SoFi Stadium</t>
+  </si>
+  <si>
+    <t>EverBank Stadium</t>
+  </si>
+  <si>
+    <t>Raymond James Stadium</t>
+  </si>
+  <si>
+    <t>Gillette Stadium</t>
+  </si>
+  <si>
+    <t>Hard Rock Stadium</t>
+  </si>
+  <si>
+    <t>NRG Stadium</t>
+  </si>
+  <si>
+    <t>Ford Field</t>
   </si>
   <si>
     <t>Huntington Bank Field</t>
   </si>
   <si>
-    <t>Highmark Stadium</t>
-  </si>
-  <si>
-    <t>Mercedes-Benz Stadium</t>
-  </si>
-  <si>
-    <t>SoFi Stadium</t>
+    <t>Paycor Stadium</t>
+  </si>
+  <si>
+    <t>Lumen Field</t>
+  </si>
+  <si>
+    <t>Allegiant Stadium</t>
+  </si>
+  <si>
+    <t>Empower Field at Mile High</t>
   </si>
   <si>
     <t>Northwest Stadium</t>
@@ -128,12 +131,6 @@
   </si>
   <si>
     <t>Acrisure Stadium</t>
-  </si>
-  <si>
-    <t>Raymond James Stadium</t>
-  </si>
-  <si>
-    <t>State Farm Stadium</t>
   </si>
 </sst>
 </file>
@@ -491,7 +488,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -513,10 +510,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -524,10 +521,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -538,7 +535,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -549,7 +546,7 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -560,7 +557,7 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -571,7 +568,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -582,7 +579,7 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -593,7 +590,7 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -604,7 +601,7 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -615,7 +612,7 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -626,7 +623,7 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -637,7 +634,7 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -645,10 +642,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -656,10 +653,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -667,10 +664,21 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>